<commit_message>
Modificação da porcentagem de conclusao do projeto
</commit_message>
<xml_diff>
--- a/Documentação/Projeto.xlsx
+++ b/Documentação/Projeto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\Estudos\APS\APS - Biometria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\Estudos\APS\APS - Biometria\Projeto\verificacaoBiometrica\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -373,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -382,6 +382,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,7 +690,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -945,6 +946,9 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -965,6 +969,9 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>0.5</v>
+      </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Atualizando porcentagem de conclusao no cronograma do projeto
</commit_message>
<xml_diff>
--- a/Documentação/Projeto.xlsx
+++ b/Documentação/Projeto.xlsx
@@ -373,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -382,7 +382,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,10 +691,13 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="59.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -725,6 +729,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -745,6 +750,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
@@ -765,6 +771,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -788,6 +795,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -811,6 +819,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -837,6 +846,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -860,6 +870,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -883,6 +894,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -906,6 +918,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -926,6 +939,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -946,7 +960,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="5">
         <v>1</v>
       </c>
       <c r="B12" t="s">
@@ -969,8 +983,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>0.5</v>
+      <c r="A13" s="5">
+        <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -992,6 +1006,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -1015,6 +1030,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -1038,6 +1054,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -1060,7 +1077,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Alterações pontuais nos arquivos
</commit_message>
<xml_diff>
--- a/Documentação/Projeto.xlsx
+++ b/Documentação/Projeto.xlsx
@@ -694,7 +694,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1033,9 +1033,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>0.25</v>
-      </c>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Atualização na porcentagem de conclusão no cronograma
</commit_message>
<xml_diff>
--- a/Documentação/Projeto.xlsx
+++ b/Documentação/Projeto.xlsx
@@ -694,7 +694,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -732,7 +732,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="A2" s="4">
+        <v>0.12</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -753,7 +755,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4">
+        <v>0.13</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
@@ -774,7 +778,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -798,7 +804,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -942,7 +950,9 @@
       </c>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="4">
+        <v>0.12</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>